<commit_message>
data scraping fix and injestion
</commit_message>
<xml_diff>
--- a/data/banks.xlsx
+++ b/data/banks.xlsx
@@ -17,8 +17,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD"/>
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -514,7 +514,7 @@
         <v>23.9</v>
       </c>
       <c r="I2" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="3">
@@ -547,7 +547,7 @@
         <v>23.5</v>
       </c>
       <c r="I3" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="4">
@@ -580,7 +580,7 @@
         <v>22.7</v>
       </c>
       <c r="I4" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="5">
@@ -613,7 +613,7 @@
         <v>24</v>
       </c>
       <c r="I5" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="6">
@@ -646,7 +646,7 @@
         <v>24</v>
       </c>
       <c r="I6" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="7">
@@ -679,7 +679,7 @@
         <v>24</v>
       </c>
       <c r="I7" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="8">
@@ -710,7 +710,7 @@
         <v>24.13</v>
       </c>
       <c r="I8" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="9">
@@ -741,7 +741,7 @@
         <v>21.5</v>
       </c>
       <c r="I9" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="10">
@@ -774,7 +774,7 @@
         <v>23.35</v>
       </c>
       <c r="I10" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="11">
@@ -805,7 +805,7 @@
         <v>22.03</v>
       </c>
       <c r="I11" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="12">
@@ -836,7 +836,7 @@
         <v>25</v>
       </c>
       <c r="I12" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="13">
@@ -867,7 +867,7 @@
         <v>23.52</v>
       </c>
       <c r="I13" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="14">
@@ -900,7 +900,7 @@
         <v>22.4</v>
       </c>
       <c r="I14" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="15">
@@ -933,7 +933,7 @@
         <v>22.2</v>
       </c>
       <c r="I15" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="16">
@@ -964,7 +964,7 @@
         <v>19.5</v>
       </c>
       <c r="I16" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="17">
@@ -995,7 +995,7 @@
         <v>24</v>
       </c>
       <c r="I17" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="18">
@@ -1026,7 +1026,7 @@
         <v>23.7</v>
       </c>
       <c r="I18" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="19">
@@ -1057,7 +1057,7 @@
         <v>22.16</v>
       </c>
       <c r="I19" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="20">
@@ -1090,7 +1090,7 @@
         <v>23</v>
       </c>
       <c r="I20" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="21">
@@ -1123,7 +1123,7 @@
         <v>19</v>
       </c>
       <c r="I21" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="22">
@@ -1154,7 +1154,7 @@
         <v>22.7</v>
       </c>
       <c r="I22" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="23">
@@ -1185,7 +1185,7 @@
         <v>21</v>
       </c>
       <c r="I23" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="24">
@@ -1218,7 +1218,7 @@
         <v>18</v>
       </c>
       <c r="I24" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="25">
@@ -1251,7 +1251,7 @@
         <v>30</v>
       </c>
       <c r="I25" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="26">
@@ -1282,7 +1282,7 @@
         <v>22.74</v>
       </c>
       <c r="I26" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="27">
@@ -1313,7 +1313,7 @@
         <v>23.76</v>
       </c>
       <c r="I27" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="28">
@@ -1344,7 +1344,7 @@
         <v>23.6</v>
       </c>
       <c r="I28" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="29">
@@ -1375,7 +1375,7 @@
         <v>23.54</v>
       </c>
       <c r="I29" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="30">
@@ -1408,7 +1408,7 @@
         <v>23</v>
       </c>
       <c r="I30" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="31">
@@ -1441,7 +1441,7 @@
         <v>23</v>
       </c>
       <c r="I31" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="32">
@@ -1472,7 +1472,7 @@
         <v>23</v>
       </c>
       <c r="I32" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="33">
@@ -1503,7 +1503,7 @@
         <v>23</v>
       </c>
       <c r="I33" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="34">
@@ -1536,7 +1536,7 @@
         <v>22.7</v>
       </c>
       <c r="I34" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="35">
@@ -1567,7 +1567,7 @@
         <v>9.140000000000001</v>
       </c>
       <c r="I35" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="36">
@@ -1598,7 +1598,7 @@
         <v>22.3</v>
       </c>
       <c r="I36" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="37">
@@ -1629,7 +1629,7 @@
         <v>23.3</v>
       </c>
       <c r="I37" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="38">
@@ -1662,7 +1662,7 @@
         <v>21.25</v>
       </c>
       <c r="I38" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="39">
@@ -1695,7 +1695,7 @@
         <v>20.15</v>
       </c>
       <c r="I39" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="40">
@@ -1726,7 +1726,7 @@
         <v>19</v>
       </c>
       <c r="I40" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="41">
@@ -1757,7 +1757,7 @@
         <v>18</v>
       </c>
       <c r="I41" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="42">
@@ -1788,7 +1788,7 @@
         <v>16</v>
       </c>
       <c r="I42" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="43">
@@ -1819,7 +1819,7 @@
         <v>22.83</v>
       </c>
       <c r="I43" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="44">
@@ -1850,7 +1850,7 @@
         <v>20.06</v>
       </c>
       <c r="I44" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="45">
@@ -1883,7 +1883,7 @@
         <v>24</v>
       </c>
       <c r="I45" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="46">
@@ -1914,7 +1914,7 @@
         <v>25</v>
       </c>
       <c r="I46" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="47">
@@ -1945,7 +1945,7 @@
         <v>25</v>
       </c>
       <c r="I47" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="48">
@@ -1978,7 +1978,7 @@
         <v>25</v>
       </c>
       <c r="I48" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="49">
@@ -2009,7 +2009,7 @@
         <v>15.1</v>
       </c>
       <c r="I49" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="50">
@@ -2040,7 +2040,7 @@
         <v>25</v>
       </c>
       <c r="I50" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="51">
@@ -2071,7 +2071,7 @@
         <v>25</v>
       </c>
       <c r="I51" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="52">
@@ -2104,7 +2104,7 @@
         <v>24.19</v>
       </c>
       <c r="I52" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="53">
@@ -2135,7 +2135,7 @@
         <v>24.5</v>
       </c>
       <c r="I53" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="54">
@@ -2166,7 +2166,7 @@
         <v>24.3</v>
       </c>
       <c r="I54" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="55">
@@ -2197,7 +2197,7 @@
         <v>24.05</v>
       </c>
       <c r="I55" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="56">
@@ -2228,7 +2228,7 @@
         <v>24</v>
       </c>
       <c r="I56" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="57">
@@ -2259,7 +2259,7 @@
         <v>18.16</v>
       </c>
       <c r="I57" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="58">
@@ -2292,7 +2292,7 @@
         <v>24</v>
       </c>
       <c r="I58" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="59">
@@ -2323,7 +2323,7 @@
         <v>20.98</v>
       </c>
       <c r="I59" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="60">
@@ -2354,7 +2354,7 @@
         <v>24</v>
       </c>
       <c r="I60" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="61">
@@ -2387,7 +2387,7 @@
         <v>24</v>
       </c>
       <c r="I61" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="62">
@@ -2418,7 +2418,7 @@
         <v>14.31</v>
       </c>
       <c r="I62" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="63">
@@ -2449,7 +2449,7 @@
         <v>24</v>
       </c>
       <c r="I63" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="64">
@@ -2480,7 +2480,7 @@
         <v>23.8</v>
       </c>
       <c r="I64" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="65">
@@ -2511,7 +2511,7 @@
         <v>23.49</v>
       </c>
       <c r="I65" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="66">
@@ -2544,7 +2544,7 @@
         <v>23.5</v>
       </c>
       <c r="I66" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="67">
@@ -2575,7 +2575,7 @@
         <v>23.5</v>
       </c>
       <c r="I67" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="68">
@@ -2606,7 +2606,7 @@
         <v>9.17</v>
       </c>
       <c r="I68" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="69">
@@ -2637,7 +2637,7 @@
         <v>23.3</v>
       </c>
       <c r="I69" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="70">
@@ -2668,7 +2668,7 @@
         <v>23.3</v>
       </c>
       <c r="I70" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="71">
@@ -2701,7 +2701,7 @@
         <v>17.69</v>
       </c>
       <c r="I71" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="72">
@@ -2732,7 +2732,7 @@
         <v>23.25</v>
       </c>
       <c r="I72" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="73">
@@ -2763,7 +2763,7 @@
         <v>23</v>
       </c>
       <c r="I73" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="74">
@@ -2794,7 +2794,7 @@
         <v>23</v>
       </c>
       <c r="I74" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="75">
@@ -2825,7 +2825,7 @@
         <v>23</v>
       </c>
       <c r="I75" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="76">
@@ -2856,7 +2856,7 @@
         <v>23</v>
       </c>
       <c r="I76" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="77">
@@ -2887,7 +2887,7 @@
         <v>23</v>
       </c>
       <c r="I77" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="78">
@@ -2918,7 +2918,7 @@
         <v>23</v>
       </c>
       <c r="I78" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="79">
@@ -2949,7 +2949,7 @@
         <v>23</v>
       </c>
       <c r="I79" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="80">
@@ -2980,7 +2980,7 @@
         <v>22.58</v>
       </c>
       <c r="I80" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="81">
@@ -3013,7 +3013,7 @@
         <v>22.89</v>
       </c>
       <c r="I81" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="82">
@@ -3044,7 +3044,7 @@
         <v>22.8</v>
       </c>
       <c r="I82" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="83">
@@ -3075,7 +3075,7 @@
         <v>22.8</v>
       </c>
       <c r="I83" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="84">
@@ -3106,7 +3106,7 @@
         <v>14.43</v>
       </c>
       <c r="I84" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="85">
@@ -3137,7 +3137,7 @@
         <v>22.7</v>
       </c>
       <c r="I85" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="86">
@@ -3170,7 +3170,7 @@
         <v>22.6</v>
       </c>
       <c r="I86" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="87">
@@ -3201,7 +3201,7 @@
         <v>22.55</v>
       </c>
       <c r="I87" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="88">
@@ -3232,7 +3232,7 @@
         <v>22.55</v>
       </c>
       <c r="I88" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="89">
@@ -3265,7 +3265,7 @@
         <v>22.51</v>
       </c>
       <c r="I89" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="90">
@@ -3298,7 +3298,7 @@
         <v>22.5</v>
       </c>
       <c r="I90" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="91">
@@ -3329,7 +3329,7 @@
         <v>22.5</v>
       </c>
       <c r="I91" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="92">
@@ -3360,7 +3360,7 @@
         <v>22.5</v>
       </c>
       <c r="I92" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="93">
@@ -3391,7 +3391,7 @@
         <v>22.5</v>
       </c>
       <c r="I93" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="94">
@@ -3422,7 +3422,7 @@
         <v>22.5</v>
       </c>
       <c r="I94" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="95">
@@ -3455,7 +3455,7 @@
         <v>22.5</v>
       </c>
       <c r="I95" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="96">
@@ -3486,7 +3486,7 @@
         <v>22.5</v>
       </c>
       <c r="I96" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="97">
@@ -3519,7 +3519,7 @@
         <v>22</v>
       </c>
       <c r="I97" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="98">
@@ -3550,7 +3550,7 @@
         <v>22</v>
       </c>
       <c r="I98" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="99">
@@ -3583,7 +3583,7 @@
         <v>22</v>
       </c>
       <c r="I99" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="100">
@@ -3614,7 +3614,7 @@
         <v>19.22</v>
       </c>
       <c r="I100" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="101">
@@ -3645,7 +3645,7 @@
         <v>22</v>
       </c>
       <c r="I101" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="102">
@@ -3676,7 +3676,7 @@
         <v>24.36</v>
       </c>
       <c r="I102" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="103">
@@ -3707,7 +3707,7 @@
         <v>22</v>
       </c>
       <c r="I103" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="104">
@@ -3740,7 +3740,7 @@
         <v>21.5</v>
       </c>
       <c r="I104" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="105">
@@ -3773,7 +3773,7 @@
         <v>21.5</v>
       </c>
       <c r="I105" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="106">
@@ -3804,7 +3804,7 @@
         <v>21.25</v>
       </c>
       <c r="I106" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="107">
@@ -3835,7 +3835,7 @@
         <v>21.15</v>
       </c>
       <c r="I107" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="108">
@@ -3866,7 +3866,7 @@
         <v>21</v>
       </c>
       <c r="I108" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="109">
@@ -3897,7 +3897,7 @@
         <v>21</v>
       </c>
       <c r="I109" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="110">
@@ -3928,7 +3928,7 @@
         <v>21</v>
       </c>
       <c r="I110" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="111">
@@ -3959,7 +3959,7 @@
         <v>21</v>
       </c>
       <c r="I111" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="112">
@@ -3990,7 +3990,7 @@
         <v>21</v>
       </c>
       <c r="I112" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="113">
@@ -4021,7 +4021,7 @@
         <v>16.01</v>
       </c>
       <c r="I113" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="114">
@@ -4054,7 +4054,7 @@
         <v>21</v>
       </c>
       <c r="I114" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="115">
@@ -4085,7 +4085,7 @@
         <v>21</v>
       </c>
       <c r="I115" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="116">
@@ -4116,7 +4116,7 @@
         <v>21</v>
       </c>
       <c r="I116" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="117">
@@ -4147,7 +4147,7 @@
         <v>21</v>
       </c>
       <c r="I117" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="118">
@@ -4178,7 +4178,7 @@
         <v>21</v>
       </c>
       <c r="I118" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="119">
@@ -4209,7 +4209,7 @@
         <v>22.61</v>
       </c>
       <c r="I119" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="120">
@@ -4240,7 +4240,7 @@
         <v>20.9</v>
       </c>
       <c r="I120" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="121">
@@ -4271,7 +4271,7 @@
         <v>20.59</v>
       </c>
       <c r="I121" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="122">
@@ -4302,7 +4302,7 @@
         <v>20.5</v>
       </c>
       <c r="I122" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="123">
@@ -4333,7 +4333,7 @@
         <v>20.5</v>
       </c>
       <c r="I123" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="124">
@@ -4364,7 +4364,7 @@
         <v>20.5</v>
       </c>
       <c r="I124" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="125">
@@ -4395,7 +4395,7 @@
         <v>20.5</v>
       </c>
       <c r="I125" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="126">
@@ -4426,7 +4426,7 @@
         <v>20.5</v>
       </c>
       <c r="I126" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="127">
@@ -4457,7 +4457,7 @@
         <v>20.4</v>
       </c>
       <c r="I127" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="128">
@@ -4488,7 +4488,7 @@
         <v>20.34</v>
       </c>
       <c r="I128" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="129">
@@ -4519,7 +4519,7 @@
         <v>20.25</v>
       </c>
       <c r="I129" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="130">
@@ -4550,7 +4550,7 @@
         <v>20.2</v>
       </c>
       <c r="I130" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="131">
@@ -4581,7 +4581,7 @@
         <v>20.1</v>
       </c>
       <c r="I131" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="132">
@@ -4612,7 +4612,7 @@
         <v>20</v>
       </c>
       <c r="I132" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="133">
@@ -4645,7 +4645,7 @@
         <v>20</v>
       </c>
       <c r="I133" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="134">
@@ -4676,7 +4676,7 @@
         <v>20</v>
       </c>
       <c r="I134" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="135">
@@ -4707,7 +4707,7 @@
         <v>20</v>
       </c>
       <c r="I135" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="136">
@@ -4738,7 +4738,7 @@
         <v>20</v>
       </c>
       <c r="I136" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="137">
@@ -4769,7 +4769,7 @@
         <v>20</v>
       </c>
       <c r="I137" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="138">
@@ -4800,7 +4800,7 @@
         <v>20</v>
       </c>
       <c r="I138" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="139">
@@ -4831,7 +4831,7 @@
         <v>20</v>
       </c>
       <c r="I139" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="140">
@@ -4862,7 +4862,7 @@
         <v>19.7</v>
       </c>
       <c r="I140" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="141">
@@ -4895,7 +4895,7 @@
         <v>19.5</v>
       </c>
       <c r="I141" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="142">
@@ -4926,7 +4926,7 @@
         <v>19.5</v>
       </c>
       <c r="I142" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="143">
@@ -4957,7 +4957,7 @@
         <v>19.5</v>
       </c>
       <c r="I143" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="144">
@@ -4990,7 +4990,7 @@
         <v>19</v>
       </c>
       <c r="I144" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="145">
@@ -5021,7 +5021,7 @@
         <v>19</v>
       </c>
       <c r="I145" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="146">
@@ -5052,7 +5052,7 @@
         <v>19</v>
       </c>
       <c r="I146" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="147">
@@ -5083,7 +5083,7 @@
         <v>19</v>
       </c>
       <c r="I147" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="148">
@@ -5114,7 +5114,7 @@
         <v>19</v>
       </c>
       <c r="I148" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="149">
@@ -5145,7 +5145,7 @@
         <v>19</v>
       </c>
       <c r="I149" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="150">
@@ -5176,7 +5176,7 @@
         <v>19</v>
       </c>
       <c r="I150" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="151">
@@ -5207,7 +5207,7 @@
         <v>19</v>
       </c>
       <c r="I151" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="152">
@@ -5240,7 +5240,7 @@
         <v>18.9</v>
       </c>
       <c r="I152" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="153">
@@ -5271,7 +5271,7 @@
         <v>18.75</v>
       </c>
       <c r="I153" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="154">
@@ -5302,7 +5302,7 @@
         <v>18.75</v>
       </c>
       <c r="I154" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="155">
@@ -5333,7 +5333,7 @@
         <v>18.75</v>
       </c>
       <c r="I155" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="156">
@@ -5364,7 +5364,7 @@
         <v>18.5</v>
       </c>
       <c r="I156" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="157">
@@ -5395,7 +5395,7 @@
         <v>18.5</v>
       </c>
       <c r="I157" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="158">
@@ -5426,7 +5426,7 @@
         <v>18</v>
       </c>
       <c r="I158" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="159">
@@ -5457,7 +5457,7 @@
         <v>18</v>
       </c>
       <c r="I159" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="160">
@@ -5488,7 +5488,7 @@
         <v>18</v>
       </c>
       <c r="I160" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="161">
@@ -5519,7 +5519,7 @@
         <v>18</v>
       </c>
       <c r="I161" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="162">
@@ -5550,7 +5550,7 @@
         <v>18</v>
       </c>
       <c r="I162" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="163">
@@ -5581,7 +5581,7 @@
         <v>18</v>
       </c>
       <c r="I163" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="164">
@@ -5612,7 +5612,7 @@
         <v>17.5</v>
       </c>
       <c r="I164" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="165">
@@ -5643,7 +5643,7 @@
         <v>17.93</v>
       </c>
       <c r="I165" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="166">
@@ -5674,7 +5674,7 @@
         <v>17</v>
       </c>
       <c r="I166" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="167">
@@ -5705,7 +5705,7 @@
         <v>17</v>
       </c>
       <c r="I167" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="168">
@@ -5736,7 +5736,7 @@
         <v>17</v>
       </c>
       <c r="I168" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="169">
@@ -5767,7 +5767,7 @@
         <v>15.97</v>
       </c>
       <c r="I169" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="170">
@@ -5800,7 +5800,7 @@
         <v>16</v>
       </c>
       <c r="I170" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="171">
@@ -5831,7 +5831,7 @@
         <v>16</v>
       </c>
       <c r="I171" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="172">
@@ -5862,7 +5862,7 @@
         <v>16</v>
       </c>
       <c r="I172" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="173">
@@ -5893,7 +5893,7 @@
         <v>16</v>
       </c>
       <c r="I173" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="174">
@@ -5924,7 +5924,7 @@
         <v>15</v>
       </c>
       <c r="I174" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="175">
@@ -5955,7 +5955,7 @@
         <v>13.5</v>
       </c>
       <c r="I175" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="176">
@@ -5986,7 +5986,7 @@
         <v>13.4</v>
       </c>
       <c r="I176" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="177">
@@ -6017,7 +6017,7 @@
         <v>10</v>
       </c>
       <c r="I177" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="178">
@@ -6048,7 +6048,7 @@
         <v>9</v>
       </c>
       <c r="I178" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="179">
@@ -6081,7 +6081,7 @@
         <v>8</v>
       </c>
       <c r="I179" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="180">
@@ -6112,7 +6112,7 @@
         <v>8</v>
       </c>
       <c r="I180" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="181">
@@ -6143,7 +6143,7 @@
         <v>8</v>
       </c>
       <c r="I181" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="182">
@@ -6174,7 +6174,7 @@
         <v>7</v>
       </c>
       <c r="I182" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="183">
@@ -6205,7 +6205,7 @@
         <v>6.5</v>
       </c>
       <c r="I183" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="184">
@@ -6236,7 +6236,7 @@
         <v>4.5</v>
       </c>
       <c r="I184" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="185">
@@ -6267,7 +6267,7 @@
         <v>4.5</v>
       </c>
       <c r="I185" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="186">
@@ -6300,7 +6300,7 @@
         <v>4.5</v>
       </c>
       <c r="I186" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="187">
@@ -6331,7 +6331,7 @@
         <v>3</v>
       </c>
       <c r="I187" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
     <row r="188">
@@ -6364,7 +6364,7 @@
         <v>2</v>
       </c>
       <c r="I188" s="2" t="n">
-        <v>45653</v>
+        <v>45653.61413774473</v>
       </c>
     </row>
   </sheetData>

</xml_diff>